<commit_message>
Attempt to make a modular Excel class for handling multiple files
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sean's Test sheet" sheetId="1" r:id="R48e21e083ea04d30"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sean's Test sheet" sheetId="1" r:id="Rebf3ea8a4d434cf9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -35,7 +35,7 @@
         <x:v>1999/01/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8477</x:v>
+        <x:v>2094</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -49,7 +49,7 @@
         <x:v>1999/02/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>4122</x:v>
+        <x:v>5517</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -63,7 +63,7 @@
         <x:v>1999/03/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>6607</x:v>
+        <x:v>9539</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -77,7 +77,7 @@
         <x:v>1999/04/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>9174</x:v>
+        <x:v>8292</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -91,7 +91,7 @@
         <x:v>1999/05/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>2477</x:v>
+        <x:v>4878</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -105,7 +105,7 @@
         <x:v>1999/06/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1685</x:v>
+        <x:v>360</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -119,7 +119,7 @@
         <x:v>1999/07/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8417</x:v>
+        <x:v>1083</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -133,7 +133,7 @@
         <x:v>1999/08/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3609</x:v>
+        <x:v>5694</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -147,7 +147,7 @@
         <x:v>1999/09/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>3562</x:v>
+        <x:v>333</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -161,7 +161,7 @@
         <x:v>1999/10/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>1812</x:v>
+        <x:v>3456</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -175,7 +175,7 @@
         <x:v>1999/11/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>4427</x:v>
+        <x:v>845</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -189,7 +189,7 @@
         <x:v>1999/12/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8711</x:v>
+        <x:v>2621</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -203,7 +203,7 @@
         <x:v>2000/01/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>6403</x:v>
+        <x:v>9145</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -217,7 +217,7 @@
         <x:v>2000/02/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>6861</x:v>
+        <x:v>3897</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -231,7 +231,7 @@
         <x:v>2000/03/01</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>8454</x:v>
+        <x:v>6421</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>